<commit_message>
fix ks-pcg change to cuadrados_medios2
</commit_message>
<xml_diff>
--- a/Números_generados.xlsx
+++ b/Números_generados.xlsx
@@ -438,7 +438,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>6944</v>
+        <v>4091</v>
       </c>
     </row>
     <row r="3">
@@ -446,7 +446,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>2191</v>
+        <v>7362</v>
       </c>
     </row>
     <row r="4">
@@ -454,7 +454,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>8004</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="5">
@@ -462,7 +462,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>640</v>
+        <v>9601</v>
       </c>
     </row>
     <row r="6">
@@ -470,7 +470,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>960</v>
+        <v>1792</v>
       </c>
     </row>
     <row r="7">
@@ -478,7 +478,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>2160</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="8">
@@ -486,7 +486,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>6656</v>
+        <v>4605</v>
       </c>
     </row>
     <row r="9">
@@ -494,7 +494,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>3023</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="10">
@@ -502,7 +502,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>1385</v>
+        <v>2436</v>
       </c>
     </row>
     <row r="11">
@@ -510,7 +510,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>9182</v>
+        <v>9340</v>
       </c>
     </row>
     <row r="12">
@@ -518,7 +518,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>3091</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="13">
@@ -526,7 +526,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>5542</v>
+        <v>5507</v>
       </c>
     </row>
     <row r="14">
@@ -534,7 +534,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>7137</v>
+        <v>3270</v>
       </c>
     </row>
     <row r="15">
@@ -542,7 +542,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>9367</v>
+        <v>6929</v>
       </c>
     </row>
     <row r="16">
@@ -550,7 +550,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>7406</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17">
@@ -558,7 +558,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>8488</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="18">
@@ -566,7 +566,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>461</v>
+        <v>4641</v>
       </c>
     </row>
     <row r="19">
@@ -574,7 +574,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>1252</v>
+        <v>5388</v>
       </c>
     </row>
     <row r="20">
@@ -582,7 +582,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>5675</v>
+        <v>305</v>
       </c>
     </row>
     <row r="21">
@@ -590,7 +590,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>2056</v>
+        <v>9302</v>
       </c>
     </row>
     <row r="22">
@@ -598,7 +598,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>2271</v>
+        <v>5272</v>
       </c>
     </row>
     <row r="23">
@@ -606,7 +606,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>1574</v>
+        <v>7939</v>
       </c>
     </row>
     <row r="24">
@@ -614,7 +614,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>4774</v>
+        <v>277</v>
       </c>
     </row>
     <row r="25">
@@ -622,7 +622,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>7910</v>
+        <v>7672</v>
       </c>
     </row>
     <row r="26">
@@ -630,7 +630,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>5681</v>
+        <v>8595</v>
       </c>
     </row>
     <row r="27">
@@ -638,7 +638,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>2737</v>
+        <v>8740</v>
       </c>
     </row>
     <row r="28">
@@ -646,7 +646,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>4911</v>
+        <v>3876</v>
       </c>
     </row>
     <row r="29">
@@ -654,7 +654,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>1179</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30">
@@ -662,7 +662,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>3900</v>
+        <v>5428</v>
       </c>
     </row>
     <row r="31">
@@ -670,7 +670,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>2100</v>
+        <v>4631</v>
       </c>
     </row>
   </sheetData>

</xml_diff>